<commit_message>
Update data for May 18 2018
</commit_message>
<xml_diff>
--- a/data/Cam_FilingPeriod.xlsx
+++ b/data/Cam_FilingPeriod.xlsx
@@ -496,7 +496,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N107"/>
+  <dimension ref="A1:N109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="C5" sqref="C5"/>
@@ -4337,6 +4337,74 @@
         <v>1</v>
       </c>
     </row>
+    <row outlineLevel="0" r="108">
+      <c r="A108" s="4">
+        <v>128</v>
+      </c>
+      <c r="B108" s="5">
+        <v>43234.9993055556</v>
+      </c>
+      <c r="C108" s="5">
+        <v>43227.9993055556</v>
+      </c>
+      <c r="E108" s="6" t="inlineStr">
+        <is>
+          <t>2018 Second Primary</t>
+        </is>
+      </c>
+      <c r="F108" s="4">
+        <v>1</v>
+      </c>
+      <c r="G108" s="4">
+        <v>1</v>
+      </c>
+      <c r="H108" s="4">
+        <v>0</v>
+      </c>
+      <c r="K108" s="5">
+        <v>43193</v>
+      </c>
+      <c r="L108" s="4">
+        <v>1</v>
+      </c>
+      <c r="M108" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="109">
+      <c r="A109" s="4">
+        <v>129</v>
+      </c>
+      <c r="B109" s="5">
+        <v>43381.9993055556</v>
+      </c>
+      <c r="C109" s="5">
+        <v>43374.9993055556</v>
+      </c>
+      <c r="E109" s="6" t="inlineStr">
+        <is>
+          <t>2018 Second Biannual</t>
+        </is>
+      </c>
+      <c r="F109" s="4">
+        <v>1</v>
+      </c>
+      <c r="G109" s="4">
+        <v>3</v>
+      </c>
+      <c r="H109" s="4">
+        <v>0</v>
+      </c>
+      <c r="K109" s="5">
+        <v>43193</v>
+      </c>
+      <c r="L109" s="4">
+        <v>1</v>
+      </c>
+      <c r="M109" s="4">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>